<commit_message>
Updated Employee Scorecards for September
</commit_message>
<xml_diff>
--- a/hiqu/Performance Evaluation/September 2024/Dev/Abid Ali.xlsx
+++ b/hiqu/Performance Evaluation/September 2024/Dev/Abid Ali.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\docs\hiqu\Performance Evaluation\ScoreCard.Arshad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\docs\hiqu\Performance Evaluation\September 2024\Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8B7CEC-62A1-4AEC-9A96-0048FEFDB946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C2575F-38F0-4146-86A3-F6A6DBEAA180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-3840" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C18F1D24-2B51-47D5-ADD3-847EF68750D1}"/>
+    <workbookView xWindow="20370" yWindow="-3840" windowWidth="29040" windowHeight="15720" xr2:uid="{C18F1D24-2B51-47D5-ADD3-847EF68750D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="103">
   <si>
     <t>Employee Name</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Diff %</t>
   </si>
   <si>
-    <t>Difference</t>
-  </si>
-  <si>
     <t>Overall Performance</t>
   </si>
   <si>
@@ -276,9 +273,6 @@
     <t>APWORKS 2024.2 - PHASE 3</t>
   </si>
   <si>
-    <t>Add Media Type/S</t>
-  </si>
-  <si>
     <t>Project Overhead</t>
   </si>
   <si>
@@ -291,12 +285,6 @@
     <t>Design</t>
   </si>
   <si>
-    <t>NEXELUS 2024.2</t>
-  </si>
-  <si>
-    <t>Production Issue</t>
-  </si>
-  <si>
     <t>Dev Manager</t>
   </si>
   <si>
@@ -318,20 +306,57 @@
     <t>Client Items</t>
   </si>
   <si>
-    <t>Google Drive integration</t>
-  </si>
-  <si>
-    <t>Broadcast Invoices</t>
+    <t>Ability to assign Employees to Roles by Media type and by Client</t>
+  </si>
+  <si>
+    <t>Ability to automatically attach additional documents to Invoice</t>
+  </si>
+  <si>
+    <t>Add Media Type/Service type/Roles</t>
+  </si>
+  <si>
+    <t>Associate vendor/stations/sites to multiple pay to</t>
+  </si>
+  <si>
+    <t>Broadcast Invoice: Invoice View UI</t>
+  </si>
+  <si>
+    <t>Broadcast Invoice: Manage Invoice Models List</t>
+  </si>
+  <si>
+    <t>Broadcast Invoice: PDF file generation</t>
+  </si>
+  <si>
+    <t>Route invoice from one company to another</t>
+  </si>
+  <si>
+    <t>Vendor Inv: Select Client on Header</t>
+  </si>
+  <si>
+    <t>Dev Support</t>
+  </si>
+  <si>
+    <t>PR-0013</t>
+  </si>
+  <si>
+    <t>Meetings, mails, communication, TFS, Interviews</t>
+  </si>
+  <si>
+    <t>Session with US team</t>
+  </si>
+  <si>
+    <t>Hours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,6 +436,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="ARIAL"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -456,7 +487,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -579,8 +610,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
@@ -588,8 +687,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -618,12 +718,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -638,9 +732,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -674,15 +765,76 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -690,22 +842,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -726,15 +866,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="Comma" xfId="5" builtinId="3"/>
     <cellStyle name="Currency 2" xfId="3" xr:uid="{8180B592-B2B1-4676-AFAD-227D0E36D85D}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{C6FF6618-242E-45B7-94CB-EA40EC999215}"/>
@@ -1078,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9386B91B-8D62-4F20-9CB7-F711303AA283}">
   <dimension ref="B2:N35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,30 +1236,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="39"/>
+      <c r="B2" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="60"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
+      <c r="C5" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
@@ -1121,11 +1267,11 @@
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
+      <c r="C6" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
@@ -1133,11 +1279,11 @@
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
+      <c r="C7" s="62" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
@@ -1145,11 +1291,11 @@
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
@@ -1157,334 +1303,338 @@
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
+      <c r="C9" s="62" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="45">
+        <v>60</v>
+      </c>
+      <c r="C10" s="63">
         <f ca="1">(_xlfn.DAYS(TODAY(),C9)/365)</f>
-        <v>1.2136986301369863</v>
-      </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
+        <v>1.2657534246575342</v>
+      </c>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
+      <c r="C11" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
     <row r="13" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="61"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="33">
+        <v>0.9</v>
+      </c>
+      <c r="E16" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="54"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="33">
+        <v>0.95</v>
+      </c>
+      <c r="J16" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="K16" s="57"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="34">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="33">
+        <v>0.8</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="54"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="33">
+        <v>0.8</v>
+      </c>
+      <c r="J17" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="K17" s="57"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="34">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="33">
+        <v>0.9</v>
+      </c>
+      <c r="E18" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="54"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="33">
+        <v>0.85</v>
+      </c>
+      <c r="J18" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18" s="57"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="34">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="33">
+        <v>0.9</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="54"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="33">
+        <v>0.8</v>
+      </c>
+      <c r="J19" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="K19" s="57"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="34">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="33">
+        <v>0.9</v>
+      </c>
+      <c r="E20" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="54"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="33">
+        <v>0.8</v>
+      </c>
+      <c r="J20" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="K20" s="57"/>
+      <c r="L20" s="58"/>
+      <c r="M20" s="34">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="33">
+        <v>0.9</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="54"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="33">
+        <v>0.95</v>
+      </c>
+      <c r="J21" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="K21" s="57"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="34">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="33">
+        <v>0.8</v>
+      </c>
+      <c r="E22" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="54"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="33">
+        <v>0.8</v>
+      </c>
+      <c r="J22" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="K22" s="57"/>
+      <c r="L22" s="58"/>
+      <c r="M22" s="34">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="33">
+        <v>0.8</v>
+      </c>
+      <c r="E23" s="53"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="33"/>
+      <c r="J23" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="K23" s="57"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="34">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="36">
-        <v>0.9</v>
-      </c>
-      <c r="E16" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="41"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="36">
-        <v>0.95</v>
-      </c>
-      <c r="J16" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="K16" s="48"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="37">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="36">
-        <v>0.8</v>
-      </c>
-      <c r="E17" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="41"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="36">
-        <v>0.8</v>
-      </c>
-      <c r="J17" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="K17" s="48"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="37">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="36">
-        <v>0.9</v>
-      </c>
-      <c r="E18" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="41"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="36">
-        <v>0.85</v>
-      </c>
-      <c r="J18" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="K18" s="48"/>
-      <c r="L18" s="49"/>
-      <c r="M18" s="37">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="36">
-        <v>0.9</v>
-      </c>
-      <c r="E19" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="41"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="36">
-        <v>0.8</v>
-      </c>
-      <c r="J19" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="K19" s="48"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="37">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="36">
-        <v>0.9</v>
-      </c>
-      <c r="E20" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="41"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="36">
-        <v>0.8</v>
-      </c>
-      <c r="J20" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="K20" s="48"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="37">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="36">
-        <v>0.9</v>
-      </c>
-      <c r="E21" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="41"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="36">
-        <v>0.95</v>
-      </c>
-      <c r="J21" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="K21" s="48"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="37">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="36">
-        <v>0.8</v>
-      </c>
-      <c r="E22" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="41"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="36">
-        <v>0.8</v>
-      </c>
-      <c r="J22" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="K22" s="48"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="37">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="36">
-        <v>0.8</v>
-      </c>
-      <c r="E23" s="40"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="36"/>
-      <c r="J23" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="K23" s="48"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="37">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="52"/>
+      <c r="N25" s="52"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="26" t="s">
+      <c r="B27" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="E27" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="F27" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="31" t="s">
+      <c r="G27" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="H27" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="H27" s="31" t="s">
+      <c r="I27" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="I27" s="26" t="s">
+      <c r="J27" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="J27" s="31" t="s">
+      <c r="K27" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="K27" s="26" t="s">
+      <c r="L27" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="L27" s="31" t="s">
+      <c r="M27" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="M27" s="26" t="s">
+      <c r="N27" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="N27" s="31" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="1">
+      <c r="B28" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="2">
+        <v>21</v>
+      </c>
+      <c r="D28" s="2">
         <v>22</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="2">
+        <v>19</v>
+      </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -1496,14 +1646,18 @@
       <c r="N28" s="1"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="1">
+      <c r="B29" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="2">
+        <v>21</v>
+      </c>
+      <c r="D29" s="2">
         <v>22</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="E29" s="2">
+        <v>19</v>
+      </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -1515,14 +1669,18 @@
       <c r="N29" s="1"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="1">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1"/>
+      <c r="B30" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -1534,14 +1692,18 @@
       <c r="N30" s="1"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="1">
+      <c r="B31" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="2">
+        <v>18</v>
+      </c>
+      <c r="D31" s="2">
         <v>22</v>
       </c>
-      <c r="E31" s="1"/>
+      <c r="E31" s="2">
+        <v>17</v>
+      </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -1553,14 +1715,18 @@
       <c r="N31" s="1"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1"/>
+      <c r="B32" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2</v>
+      </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -1572,14 +1738,18 @@
       <c r="N32" s="1"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="1">
+      <c r="B33" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
         <v>1</v>
       </c>
-      <c r="E33" s="1"/>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -1591,14 +1761,18 @@
       <c r="N33" s="1"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="1">
-        <v>0</v>
-      </c>
-      <c r="E34" s="1"/>
+      <c r="B34" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -1610,14 +1784,18 @@
       <c r="N34" s="1"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="1">
-        <v>0</v>
-      </c>
-      <c r="E35" s="1"/>
+      <c r="B35" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="2">
+        <v>3</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>2</v>
+      </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -1630,6 +1808,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
     <mergeCell ref="B25:N25"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
@@ -1646,17 +1835,6 @@
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="C16:C23">
@@ -1758,205 +1936,212 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91243861-FD89-470C-9D9D-D3C0781A3547}">
-  <dimension ref="B2:W18"/>
+  <dimension ref="B2:X27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="6" width="9.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="57.85546875" customWidth="1"/>
+    <col min="4" max="5" width="9.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="6"/>
-    <col min="11" max="11" width="6.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.28515625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="1.7109375" style="6" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" style="6" customWidth="1"/>
-    <col min="19" max="19" width="2.28515625" style="6" customWidth="1"/>
-    <col min="20" max="22" width="9.28515625" style="6"/>
-    <col min="23" max="23" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.140625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" style="6"/>
+    <col min="12" max="12" width="6.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.28515625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="1.7109375" style="6" customWidth="1"/>
+    <col min="19" max="19" width="9.7109375" style="44" customWidth="1"/>
+    <col min="20" max="20" width="2.28515625" style="6" customWidth="1"/>
+    <col min="21" max="23" width="9.28515625" style="6"/>
+    <col min="24" max="24" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="52" t="s">
+    <row r="2" spans="2:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B2" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="52"/>
-      <c r="W2" s="52"/>
-    </row>
-    <row r="3" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="51"/>
-      <c r="U3" s="51"/>
-      <c r="V3" s="51"/>
-      <c r="W3" s="51"/>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B4" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53"/>
-      <c r="N4" s="53"/>
-      <c r="O4" s="53"/>
-      <c r="P4" s="53"/>
-      <c r="Q4" s="53"/>
-      <c r="R4" s="53"/>
-      <c r="S4" s="53"/>
-      <c r="T4" s="53"/>
-      <c r="U4" s="53"/>
-      <c r="V4" s="53"/>
-      <c r="W4" s="53"/>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="66"/>
+      <c r="X2" s="66"/>
+    </row>
+    <row r="3" spans="2:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
+      <c r="X3" s="65"/>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B4" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="67"/>
+      <c r="O4" s="67"/>
+      <c r="P4" s="67"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="67"/>
+      <c r="V4" s="67"/>
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="68" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="58" t="s">
-        <v>82</v>
-      </c>
-      <c r="I6" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="J6" s="57" t="s">
+      <c r="I6" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="51"/>
+      <c r="K6" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
-      <c r="N6" s="57" t="s">
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
+      <c r="O6" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="O6" s="57"/>
-      <c r="P6" s="57"/>
-      <c r="R6" s="14" t="s">
+      <c r="P6" s="71"/>
+      <c r="Q6" s="71"/>
+      <c r="S6" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="T6" s="54" t="s">
+      <c r="U6" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="U6" s="55"/>
-      <c r="V6" s="55"/>
-      <c r="W6" s="56"/>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V6" s="69"/>
+      <c r="W6" s="69"/>
+      <c r="X6" s="70"/>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="13"/>
-      <c r="D7" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="G7" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="12" t="s">
+      <c r="D7" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" s="75"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="L7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="M7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="O7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="P7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="P7" s="12" t="s">
+      <c r="Q7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="R7" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="T7" s="12" t="s">
+      <c r="S7" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="U7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="V7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="U7" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="V7" s="12" t="s">
+      <c r="W7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="W7" s="12" t="s">
+      <c r="X7" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B8" s="33" t="s">
-        <v>78</v>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B8" s="30" t="s">
+        <v>77</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="5"/>
@@ -1964,55 +2149,50 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="9"/>
-      <c r="N8" s="2"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="9"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="T8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="9"/>
+      <c r="S8" s="41"/>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
-      <c r="W8" s="9"/>
-    </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="W8" s="2"/>
+      <c r="X8" s="9"/>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
-      <c r="C9" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
+      <c r="C9" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
       <c r="H9" s="5">
-        <v>2</v>
-      </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="16">
-        <f t="shared" ref="L9" si="0">IF(J9=0,0,(K9-J9)/J9)</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="2">
-        <v>0</v>
-      </c>
-      <c r="O9" s="2">
-        <v>0</v>
-      </c>
-      <c r="P9" s="16">
-        <f t="shared" ref="P9" si="1">IF(N9=0,0,(O9-N9)/N9)</f>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="16">
-        <f>IF((J9+N9)=0,1,((K9+O9)-(J9+N9))/(J9+N9))</f>
-        <v>1</v>
-      </c>
-      <c r="T9" s="2">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="I9" s="45"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="14">
+        <f t="shared" ref="M9" si="0">IF(K9=0,0,(L9-K9)/K9)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="14">
+        <f t="shared" ref="Q9" si="1">IF(O9=0,0,(P9-O9)/O9)</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="8"/>
+      <c r="S9" s="41">
+        <f>D9+E9+F9+G9+H9+I9+L9+P9</f>
+        <v>3</v>
       </c>
       <c r="U9" s="2">
         <v>0</v>
@@ -2020,314 +2200,599 @@
       <c r="V9" s="2">
         <v>0</v>
       </c>
-      <c r="W9" s="9">
-        <f>SUM(T9:V9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="W9" s="2">
+        <v>0</v>
+      </c>
+      <c r="X9" s="9">
+        <f>SUM(U9:W9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
-      <c r="C10" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
+      <c r="C10" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
       <c r="H10" s="5">
-        <v>1</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="16"/>
-      <c r="N10" s="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="I10" s="45"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="14"/>
       <c r="O10" s="2"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="16"/>
-      <c r="T10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="41">
+        <f t="shared" ref="S10:S24" si="2">D10+E10+F10+G10+H10+I10+L10+P10</f>
+        <v>0.5</v>
+      </c>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
-      <c r="W10" s="9"/>
-    </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="W10" s="2"/>
+      <c r="X10" s="9"/>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
-      <c r="C11" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
+      <c r="C11" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
       <c r="H11" s="5">
         <v>2</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="16"/>
-      <c r="N11" s="2"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="14"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="16"/>
-      <c r="T11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="41">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
-      <c r="W11" s="9"/>
-    </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="W11" s="2"/>
+      <c r="X11" s="9"/>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="C12" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="5">
         <v>1</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="17"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="18"/>
-      <c r="R12" s="9"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="18"/>
-    </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B13" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="14"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="41">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="9"/>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="5">
+        <v>2</v>
+      </c>
+      <c r="I13" s="45"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="14"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="41">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
-      <c r="W13" s="9"/>
-    </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="W13" s="2"/>
+      <c r="X13" s="9"/>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="16">
-        <f t="shared" ref="L14" si="2">IF(J14=0,0,(K14-J14)/J14)</f>
-        <v>0</v>
-      </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2">
-        <v>0</v>
-      </c>
-      <c r="O14" s="2">
-        <v>26</v>
-      </c>
-      <c r="P14" s="16">
-        <f>(O14-N14)/IF(N14=0,O14,N14)</f>
-        <v>1</v>
-      </c>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="16">
-        <f>IF((J14+N14)=0,1,((K14+O14)-(J14+N14))/(J14+N14))</f>
-        <v>1</v>
-      </c>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2">
-        <v>1</v>
+      <c r="C14" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="5">
+        <v>2</v>
+      </c>
+      <c r="I14" s="45"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="14"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="41">
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
-      <c r="W14" s="9"/>
-    </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B15" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="9"/>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="5">
+        <v>5</v>
+      </c>
+      <c r="I15" s="45"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="2">
+        <v>5</v>
+      </c>
+      <c r="M15" s="14">
+        <f t="shared" ref="M15" si="3">IF(K15=0,0,(L15-K15)/K15)</f>
+        <v>0</v>
+      </c>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="41">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
-      <c r="W15" s="9"/>
-    </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="W15" s="2"/>
+      <c r="X15" s="9"/>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="16">
-        <f t="shared" ref="L16" si="3">IF(J16=0,0,(K16-J16)/J16)</f>
-        <v>0</v>
-      </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2">
-        <v>0</v>
-      </c>
-      <c r="O16" s="2">
-        <v>9</v>
-      </c>
-      <c r="P16" s="16">
-        <f>(O16-N16)/IF(N16=0,O16,N16)</f>
+      <c r="C16" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="17">
         <v>1</v>
       </c>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="16">
-        <f>IF((J16+N16)=0,1,((K16+O16)-(J16+N16))/(J16+N16))</f>
+      <c r="I16" s="46"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="15"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="41">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2">
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="16"/>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I17" s="46"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="15"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="41">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="16"/>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="2">
         <v>1</v>
       </c>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="9"/>
-    </row>
-    <row r="17" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="60" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21">
-        <f>SUM(D8:D16)</f>
+      <c r="E18" s="2">
+        <v>13.5</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="15"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="16"/>
+      <c r="S18" s="41">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="16"/>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B19" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="41"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="9"/>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B20" s="30"/>
+      <c r="C20" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2">
         <v>1</v>
       </c>
-      <c r="E17" s="21">
-        <f>SUM(E8:E16)</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="21">
-        <f>SUM(F8:F16)</f>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="41">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="9"/>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="14">
+        <f t="shared" ref="M21" si="4">IF(K21=0,0,(L21-K21)/K21)</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2">
+        <v>16</v>
+      </c>
+      <c r="Q21" s="14">
+        <f t="shared" ref="Q21" si="5">IF(O21=0,0,(P21-O21)/O21)</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="2"/>
+      <c r="S21" s="41">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="9"/>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B22" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="41"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7"/>
+      <c r="X22" s="16"/>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="7">
+        <v>21.5</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="41">
+        <f t="shared" si="2"/>
+        <v>21.5</v>
+      </c>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="16"/>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="7">
+        <v>11.2</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="41">
+        <f t="shared" si="2"/>
+        <v>11.2</v>
+      </c>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="16"/>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="42"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="16"/>
+    </row>
+    <row r="26" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="19">
+        <f>SUM(D8:D25)</f>
+        <v>33.700000000000003</v>
+      </c>
+      <c r="E26" s="19">
+        <f t="shared" ref="E26:M26" si="6">SUM(E8:E25)</f>
+        <v>14.5</v>
+      </c>
+      <c r="F26" s="19">
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
-      <c r="G17" s="21">
-        <f>SUM(G8:G16)</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="21">
-        <f>SUM(H8:H16)</f>
+      <c r="G26" s="19">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="19">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="I26" s="49">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="51"/>
+      <c r="K26" s="50">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="19">
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="I17" s="21">
-        <f>SUM(I8:I16)</f>
-        <v>0</v>
-      </c>
-      <c r="J17" s="21">
-        <f>SUM(J8:J16)</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="21">
-        <f>SUM(K8:K16)</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="22">
-        <f t="shared" ref="L17" si="4">IF(J17=0,0,(K17-J17)/J17)</f>
-        <v>0</v>
-      </c>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21">
-        <f>SUM(N8:N16)</f>
-        <v>0</v>
-      </c>
-      <c r="O17" s="21">
-        <f>SUM(O8:O16)</f>
-        <v>35</v>
-      </c>
-      <c r="P17" s="22">
-        <f t="shared" ref="P17" si="5">IF(N17=0,0,(O17-N17)/N17)</f>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21">
-        <f>SUM(T8:T16)</f>
-        <v>2</v>
-      </c>
-      <c r="U17" s="21">
-        <f>SUM(U8:U16)</f>
-        <v>0</v>
-      </c>
-      <c r="V17" s="21">
-        <f>SUM(V8:V16)</f>
-        <v>0</v>
-      </c>
-      <c r="W17" s="21">
-        <f>SUM(W8:W16)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="M26" s="19">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19">
+        <f>SUM(O8:O25)</f>
+        <v>0</v>
+      </c>
+      <c r="P26" s="19">
+        <f>SUM(P8:P25)</f>
+        <v>16</v>
+      </c>
+      <c r="Q26" s="19">
+        <f>SUM(Q8:Q25)</f>
+        <v>0</v>
+      </c>
+      <c r="R26" s="19"/>
+      <c r="S26" s="43">
+        <f>SUM(S8:S25)</f>
+        <v>88.7</v>
+      </c>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19">
+        <f>SUM(U8:U25)</f>
+        <v>0</v>
+      </c>
+      <c r="V26" s="19">
+        <f>SUM(V8:V25)</f>
+        <v>0</v>
+      </c>
+      <c r="W26" s="19">
+        <f>SUM(W8:W25)</f>
+        <v>0</v>
+      </c>
+      <c r="X26" s="19">
+        <f>SUM(X8:X25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B3:W3"/>
-    <mergeCell ref="B2:W2"/>
-    <mergeCell ref="B4:W4"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="B3:X3"/>
+    <mergeCell ref="B2:X2"/>
+    <mergeCell ref="B4:X4"/>
+    <mergeCell ref="U6:X6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="O6:Q6"/>
     <mergeCell ref="D6:G6"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="H6:H7"/>
   </mergeCells>
-  <conditionalFormatting sqref="T9">
+  <conditionalFormatting sqref="U9:U13">
     <cfRule type="expression" priority="3">
-      <formula>T9/$W9</formula>
+      <formula>U9/$X9</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>